<commit_message>
updated competition results templates to jxls3
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/templates/competitionResults/Results-A4.xlsx
+++ b/owlcms/src/main/resources/templates/competitionResults/Results-A4.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottgonzalez/Projects/Misc/owlcms4/owlcms/src/main/resources/templates/competitionResults/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\templates\competitionResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30680D57-7C78-4643-B712-7B4F38245AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4811450E-7358-4C46-BCBD-83EBA73A3766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="500" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="2235" windowWidth="23985" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$7:$U$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Results!$A$7:$U$10</definedName>
     <definedName name="AFF.">Results!#REF!</definedName>
     <definedName name="Affiliation">Results!#REF!</definedName>
     <definedName name="Barre">#REF!</definedName>
@@ -25,7 +25,7 @@
     <definedName name="CategoryFilter">Results!#REF!</definedName>
     <definedName name="CLUB">Results!#REF!</definedName>
     <definedName name="Collet">#REF!</definedName>
-    <definedName name="_xlnm.Criteria" localSheetId="0">Results!$A$1:$CF$98</definedName>
+    <definedName name="_xlnm.Criteria" localSheetId="0">Results!$A$1:$CF$91</definedName>
     <definedName name="demandé">Results!#REF!</definedName>
     <definedName name="dernier">Results!#REF!</definedName>
     <definedName name="essais">Results!#REF!</definedName>
@@ -37,9 +37,9 @@
     <definedName name="InactiveGroupFilter">Results!#REF!</definedName>
     <definedName name="isSnatch">Results!#REF!</definedName>
     <definedName name="lbParKg">Results!#REF!</definedName>
-    <definedName name="LignesCalculs">Results!$24:$24</definedName>
+    <definedName name="LignesCalculs">Results!$17:$17</definedName>
     <definedName name="LignesEntête">Results!$1:$5</definedName>
-    <definedName name="LignesOfficiels">Results!#REF!</definedName>
+    <definedName name="LignesOfficiels">Results!$16:$16</definedName>
     <definedName name="M_F">Results!#REF!</definedName>
     <definedName name="NAIS.">Results!#REF!</definedName>
     <definedName name="NbCollet">#REF!</definedName>
@@ -70,11 +70,83 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Jean-François Lamy</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{5464D8D0-CD5E-425C-A581-A77008842DB5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>jx:area(lastCell="V15")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0" xr:uid="{CEBD2170-0D1A-40A3-B9D6-62E3599ECF09}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>jx:each(items="athletes" var="group" groupBy="group.categorySortCode" groupOrder="ASC" lastCell="V10")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{F0A7DC28-4FBA-4A0F-B1F3-C337DC82D113}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>jx:each(items="group.items" var="l"  varIndex="lifterLoop" lastCell="V10")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{970BB391-BC34-4352-A877-A2663ADBC3A4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>jx:if(condition="records != null" lastCell="V15")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{1E324CE8-95D7-4732-87D4-D0D1EB5131F4}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>jx:each(items="records" var="r" lastCell="V15")</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="80">
-  <si>
-    <t>&lt;/jx:forEach&gt;</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>${l.lotNumber}</t>
   </si>
@@ -97,220 +169,205 @@
     <t>${l.total}</t>
   </si>
   <si>
+    <t>${l.bestSnatch}</t>
+  </si>
+  <si>
+    <t>${l.bestCleanJerk}</t>
+  </si>
+  <si>
+    <t>${l.snatch1AsInteger}</t>
+  </si>
+  <si>
+    <t>${l.snatch2AsInteger}</t>
+  </si>
+  <si>
+    <t>${l.snatch3AsInteger}</t>
+  </si>
+  <si>
+    <t>${l.cleanJerk1AsInteger}</t>
+  </si>
+  <si>
+    <t>${l.cleanJerk2AsInteger}</t>
+  </si>
+  <si>
+    <t>${l.cleanJerk3AsInteger}</t>
+  </si>
+  <si>
+    <t>${l.bodyWeight}</t>
+  </si>
+  <si>
+    <t>${competition.competitionName}</t>
+  </si>
+  <si>
+    <t>${competition.competitionCity}</t>
+  </si>
+  <si>
+    <t>${competition.competitionOrganizer}</t>
+  </si>
+  <si>
+    <t>${competition.federation}</t>
+  </si>
+  <si>
+    <t>${competition.federationAddress}</t>
+  </si>
+  <si>
+    <t>${competition.federationWebSite}</t>
+  </si>
+  <si>
+    <t>${competition.competitionSite}</t>
+  </si>
+  <si>
+    <t>${competition.federationEMail}</t>
+  </si>
+  <si>
+    <t>${l.startNumber}</t>
+  </si>
+  <si>
+    <t>${l.formattedBirth}</t>
+  </si>
+  <si>
+    <t>${t.get("Competition.competitionName")} :</t>
+  </si>
+  <si>
+    <t>${t.get("Competition.competitionSite")} :</t>
+  </si>
+  <si>
+    <t>${t.get("Competition.competitionDate")} :</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ${t.get("Competition.competitionCity")} : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${t.get("Competition.competitionOrganizer")} : </t>
+  </si>
+  <si>
+    <t>${t.get("LastName")}</t>
+  </si>
+  <si>
+    <t>${t.get("FirstName")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.Category")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.BodyWeight")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.Team")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.Birth")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.Snatch")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.Clean_and_Jerk")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.Membership")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.Start")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.Lot")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.Best")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.Snatch_abbrev")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.Total")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.Rank")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.CJ_abbrev")}</t>
+  </si>
+  <si>
+    <t>${group.item.category}</t>
+  </si>
+  <si>
+    <t>${competition.localizedCompetitionDate}</t>
+  </si>
+  <si>
+    <t>${r.recordFederation}</t>
+  </si>
+  <si>
+    <t>${r.recordName}</t>
+  </si>
+  <si>
+    <t>${r.recordValue}</t>
+  </si>
+  <si>
+    <t>${r.nation}</t>
+  </si>
+  <si>
+    <t>${r.recordDateAsString}</t>
+  </si>
+  <si>
+    <t>${r.groupNameString}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ${r.birth}</t>
+  </si>
+  <si>
+    <t>${t.get("Preparation.Records")}</t>
+  </si>
+  <si>
+    <t>${t.get("Group")}</t>
+  </si>
+  <si>
+    <t>${t.get("Name")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.RecordName")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.RecordWeight")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.RecordDate")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.RecordAgeGroup")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.RecordFederation")}</t>
+  </si>
+  <si>
+    <t>${t.get("Results.RecordKind")}</t>
+  </si>
+  <si>
+    <t>${r.bwCatString}</t>
+  </si>
+  <si>
+    <t>${r.ageGrp} ${r.gender}</t>
+  </si>
+  <si>
+    <t>${r.resAthleteName}</t>
+  </si>
+  <si>
+    <t>${r.resRecordLift}</t>
+  </si>
+  <si>
+    <t>${l.totalRank &lt; 0 ? "inv." : (l.totalRank &gt; 0 ? l.totalRank : "" )}</t>
+  </si>
+  <si>
+    <t>${l.qPoints}</t>
+  </si>
+  <si>
     <t>${l.sinclair}</t>
   </si>
   <si>
-    <t>${l.bestSnatch}</t>
-  </si>
-  <si>
-    <t>${l.bestCleanJerk}</t>
-  </si>
-  <si>
-    <t>${l.snatch1AsInteger}</t>
-  </si>
-  <si>
-    <t>${l.snatch2AsInteger}</t>
-  </si>
-  <si>
-    <t>${l.snatch3AsInteger}</t>
-  </si>
-  <si>
-    <t>${l.cleanJerk1AsInteger}</t>
-  </si>
-  <si>
-    <t>${l.cleanJerk2AsInteger}</t>
-  </si>
-  <si>
-    <t>${l.cleanJerk3AsInteger}</t>
-  </si>
-  <si>
-    <t>${l.bodyWeight}</t>
-  </si>
-  <si>
-    <t>${competition.competitionName}</t>
-  </si>
-  <si>
-    <t>${competition.competitionCity}</t>
-  </si>
-  <si>
-    <t>${competition.competitionOrganizer}</t>
-  </si>
-  <si>
-    <t>${competition.federation}</t>
-  </si>
-  <si>
-    <t>${competition.federationAddress}</t>
-  </si>
-  <si>
-    <t>${competition.federationWebSite}</t>
-  </si>
-  <si>
-    <t>${competition.competitionSite}</t>
-  </si>
-  <si>
-    <t>${competition.federationEMail}</t>
-  </si>
-  <si>
-    <t>${l.startNumber}</t>
-  </si>
-  <si>
-    <t>${l.robi}</t>
-  </si>
-  <si>
-    <t>${l.formattedBirth}</t>
-  </si>
-  <si>
-    <t>${t.get("Competition.competitionName")} :</t>
-  </si>
-  <si>
-    <t>${t.get("Competition.competitionSite")} :</t>
-  </si>
-  <si>
-    <t>${t.get("Competition.competitionDate")} :</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ${t.get("Competition.competitionCity")} : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">${t.get("Competition.competitionOrganizer")} : </t>
-  </si>
-  <si>
-    <t>${t.get("LastName")}</t>
-  </si>
-  <si>
-    <t>${t.get("FirstName")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.Category")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.BodyWeight")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.Team")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.Birth")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.Snatch")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.Clean_and_Jerk")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.Membership")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.Start")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.Lot")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.Best")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.Snatch_abbrev")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.Total")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.Rank")}</t>
+    <t>${t.get("Qpoints")}</t>
   </si>
   <si>
     <t>${t.get("Results.Sinclair")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.CJ_abbrev")}</t>
-  </si>
-  <si>
-    <t>${t.get("robi")}</t>
-  </si>
-  <si>
-    <t>${group.item.category}</t>
-  </si>
-  <si>
-    <t>&lt;jx:forEach items="${group.items}" var="l" varStatus="lifterLoop"&gt;</t>
-  </si>
-  <si>
-    <t>${competition.localizedCompetitionDate}</t>
-  </si>
-  <si>
-    <t>&lt;jx:forEach items="${athletes}" groupBy="displayCategory"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;jx:forEach items="${records}" var="r"&gt;</t>
-  </si>
-  <si>
-    <t>${r.recordFederation}</t>
-  </si>
-  <si>
-    <t>${r.recordName}</t>
-  </si>
-  <si>
-    <t>${r.recordValue}</t>
-  </si>
-  <si>
-    <t>${r.nation}</t>
-  </si>
-  <si>
-    <t>${r.recordDateAsString}</t>
-  </si>
-  <si>
-    <t>${r.groupNameString}</t>
-  </si>
-  <si>
-    <t>&lt;/jx:if&gt;</t>
-  </si>
-  <si>
-    <t>&lt;jx:if test="${records != null}"&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ${r.birth}</t>
-  </si>
-  <si>
-    <t>${t.get("Preparation.Records")}</t>
-  </si>
-  <si>
-    <t>${t.get("Group")}</t>
-  </si>
-  <si>
-    <t>${t.get("Name")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.RecordName")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.RecordWeight")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.RecordDate")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.RecordAgeGroup")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.RecordFederation")}</t>
-  </si>
-  <si>
-    <t>${t.get("Results.RecordKind")}</t>
-  </si>
-  <si>
-    <t>${r.bwCatString}</t>
-  </si>
-  <si>
-    <t>${r.ageGrp} ${r.gender}</t>
-  </si>
-  <si>
-    <t>${r.resAthleteName}</t>
-  </si>
-  <si>
-    <t>${r.resRecordLift}</t>
-  </si>
-  <si>
-    <t>${l.totalRank &lt; 0 ? "inv." : (l.totalRank &gt; 0 ? l.totalRank : "" )}</t>
   </si>
 </sst>
 </file>
@@ -325,7 +382,7 @@
     <numFmt numFmtId="168" formatCode="0.000;;\-"/>
     <numFmt numFmtId="169" formatCode="0;\-;\-"/>
   </numFmts>
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -413,6 +470,12 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -484,12 +547,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -506,6 +563,18 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -864,7 +933,7 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -872,7 +941,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -883,9 +952,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -915,6 +981,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -943,6 +1013,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
@@ -969,47 +1046,28 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1018,15 +1076,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1036,58 +1091,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="12" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="12" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1099,17 +1126,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="12" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="14" xfId="12" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="15" fillId="0" borderId="14" xfId="12" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="12" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1123,14 +1150,37 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="15" xfId="12" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="15" xfId="12" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -1152,11 +1202,9 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1206,39 +1254,7 @@
     <cellStyle name="Titre de la feuille" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="34"/>
-          <bgColor indexed="13"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1691,297 +1707,348 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Feuil4">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X124"/>
+  <dimension ref="A1:X117"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="1" customWidth="1"/>
-    <col min="11" max="13" width="7.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.6640625" customWidth="1"/>
-    <col min="15" max="15" width="7.6640625" style="3" customWidth="1"/>
-    <col min="16" max="18" width="7.6640625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="7.6640625" customWidth="1"/>
-    <col min="20" max="20" width="8.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="8.1640625" style="1" customWidth="1"/>
-    <col min="22" max="23" width="10.1640625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="8.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="1" customWidth="1"/>
+    <col min="11" max="13" width="7.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" customWidth="1"/>
+    <col min="15" max="15" width="7.7109375" style="3" customWidth="1"/>
+    <col min="16" max="18" width="7.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="7.7109375" customWidth="1"/>
+    <col min="20" max="20" width="8.42578125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="8.140625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="10.140625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="8.140625" style="1" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="38"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="13"/>
+      <c r="J1" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="99" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="99"/>
+      <c r="R1" s="99"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+    </row>
+    <row r="2" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="4"/>
+      <c r="J2" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="91"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="S2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="45"/>
+      <c r="U2" s="45"/>
+    </row>
+    <row r="3" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="14"/>
-      <c r="J1" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="4" t="s">
+      <c r="B3" s="47"/>
+      <c r="J3" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="98" t="s">
+        <v>48</v>
+      </c>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="35"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="38"/>
-    </row>
-    <row r="2" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="5"/>
-      <c r="J2" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="42"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="S2" s="47" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-    </row>
-    <row r="3" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
+      <c r="T3" s="50"/>
+      <c r="U3" s="50"/>
+      <c r="V3" s="83"/>
+    </row>
+    <row r="4" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="J3" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="101" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" s="101"/>
-      <c r="M3" s="101"/>
-      <c r="N3" s="101"/>
-      <c r="O3" s="101"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="54"/>
-    </row>
-    <row r="4" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="49" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="9"/>
+      <c r="B4" s="46"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="92"/>
       <c r="L4"/>
       <c r="M4" s="3"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="Q4"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="55"/>
-    </row>
-    <row r="5" spans="1:24" ht="6" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="97" t="s">
+      <c r="R4" s="24"/>
+      <c r="S4" s="51"/>
+    </row>
+    <row r="5" spans="1:24" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="94" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="106"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="O6" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="P6" s="106"/>
+      <c r="Q6" s="95"/>
+      <c r="R6" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" s="104" t="s">
+        <v>44</v>
+      </c>
+      <c r="T6" s="102" t="s">
+        <v>45</v>
+      </c>
+      <c r="U6" s="100" t="s">
+        <v>72</v>
+      </c>
+      <c r="V6" s="100" t="s">
+        <v>73</v>
+      </c>
+      <c r="X6"/>
+    </row>
+    <row r="7" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="L6" s="110"/>
-      <c r="M6" s="98"/>
-      <c r="N6" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="O6" s="97" t="s">
+      <c r="C7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="P6" s="110"/>
-      <c r="Q6" s="98"/>
-      <c r="R6" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="S6" s="108" t="s">
+      <c r="D7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="95"/>
+      <c r="G7" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="10">
+        <v>1</v>
+      </c>
+      <c r="L7" s="10">
+        <v>2</v>
+      </c>
+      <c r="M7" s="10">
+        <v>3</v>
+      </c>
+      <c r="N7" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" s="10">
+        <v>1</v>
+      </c>
+      <c r="P7" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="10">
+        <v>3</v>
+      </c>
+      <c r="R7" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="S7" s="105"/>
+      <c r="T7" s="103"/>
+      <c r="U7" s="101"/>
+      <c r="V7" s="101"/>
+    </row>
+    <row r="8" spans="1:24" s="21" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="55"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="57"/>
+      <c r="V8" s="84"/>
+    </row>
+    <row r="9" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="58" t="s">
         <v>47</v>
       </c>
-      <c r="T6" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="U6" s="102" t="s">
-        <v>49</v>
-      </c>
-      <c r="V6" s="104" t="s">
-        <v>51</v>
-      </c>
-      <c r="X6"/>
-    </row>
-    <row r="7" spans="1:24" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="97" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="98"/>
-      <c r="G7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" s="11">
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="60"/>
+      <c r="G9" s="60"/>
+      <c r="H9" s="60"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="60"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="60"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="60"/>
+      <c r="R9" s="60"/>
+      <c r="S9" s="60"/>
+      <c r="T9" s="60"/>
+      <c r="U9" s="60"/>
+      <c r="V9" s="93"/>
+      <c r="X9"/>
+    </row>
+    <row r="10" spans="1:24" s="21" customFormat="1" ht="21.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="L7" s="11">
+      <c r="B10" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="M7" s="11">
+      <c r="E10" s="96" t="s">
         <v>3</v>
       </c>
-      <c r="N7" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="O7" s="11">
-        <v>1</v>
-      </c>
-      <c r="P7" s="11">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="11">
-        <v>3</v>
-      </c>
-      <c r="R7" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="S7" s="109"/>
-      <c r="T7" s="107"/>
-      <c r="U7" s="103"/>
-      <c r="V7" s="105"/>
-    </row>
-    <row r="8" spans="1:24" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="61"/>
-    </row>
-    <row r="9" spans="1:24" s="20" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="59"/>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="61"/>
-    </row>
-    <row r="10" spans="1:24" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="62" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="64"/>
-      <c r="N10" s="64"/>
-      <c r="O10" s="64"/>
-      <c r="P10" s="64"/>
-      <c r="Q10" s="64"/>
-      <c r="R10" s="64"/>
-      <c r="S10" s="64"/>
-      <c r="T10" s="64"/>
-      <c r="U10" s="64"/>
-      <c r="V10" s="65"/>
-      <c r="X10"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
-        <v>53</v>
-      </c>
+      <c r="F10" s="97"/>
+      <c r="G10" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="M10" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="O10" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="P10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="R10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="S10" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="T10" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="U10" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="V10" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11"/>
       <c r="G11"/>
       <c r="H11"/>
       <c r="I11"/>
-      <c r="J11"/>
       <c r="K11"/>
       <c r="L11"/>
       <c r="M11"/>
@@ -1991,664 +2058,482 @@
       <c r="R11"/>
       <c r="T11"/>
       <c r="U11"/>
-      <c r="V11"/>
+      <c r="V11" s="85"/>
       <c r="W11"/>
       <c r="X11"/>
     </row>
-    <row r="12" spans="1:24" s="20" customFormat="1" ht="21.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="99" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="100"/>
-      <c r="G12" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="58" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" s="56" t="s">
-        <v>28</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="M12" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="N12" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="O12" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="P12" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q12" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="R12" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="S12" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="T12" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="U12" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="V12" s="22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13"/>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-      <c r="O13"/>
-      <c r="P13"/>
-      <c r="Q13"/>
-      <c r="R13"/>
-      <c r="T13"/>
-      <c r="U13"/>
-      <c r="V13"/>
-      <c r="W13"/>
-      <c r="X13"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14"/>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="K14"/>
-      <c r="L14"/>
-      <c r="M14"/>
-      <c r="O14"/>
-      <c r="P14"/>
-      <c r="Q14"/>
-      <c r="R14"/>
-      <c r="T14"/>
-      <c r="U14"/>
-      <c r="V14"/>
-      <c r="W14"/>
-      <c r="X14"/>
-    </row>
-    <row r="15" spans="1:24" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B15"/>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
-      <c r="R15"/>
-      <c r="T15"/>
-      <c r="U15"/>
-      <c r="V15"/>
-      <c r="W15"/>
-      <c r="X15"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
+    <row r="12" spans="1:24" s="37" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="J12" s="38"/>
+      <c r="V12" s="86"/>
+    </row>
+    <row r="13" spans="1:24" s="37" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="62"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="68"/>
+      <c r="Q13" s="68"/>
+      <c r="R13" s="68"/>
+      <c r="S13" s="62"/>
+      <c r="T13" s="62"/>
+      <c r="U13" s="68"/>
+      <c r="V13" s="87"/>
+    </row>
+    <row r="14" spans="1:24" s="80" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+      <c r="A14" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="72"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="75" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="76" t="s">
         <v>64</v>
       </c>
-      <c r="B16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16"/>
-      <c r="R16"/>
-      <c r="T16"/>
-      <c r="U16"/>
-      <c r="V16"/>
-      <c r="W16"/>
-      <c r="X16"/>
-    </row>
-    <row r="17" spans="1:24" s="33" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A17" s="33" t="s">
+      <c r="H14" s="77"/>
+      <c r="I14" s="74" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="71" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" s="78"/>
+      <c r="L14" s="72"/>
+      <c r="M14" s="73"/>
+      <c r="N14" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" s="72"/>
+      <c r="P14" s="79"/>
+      <c r="Q14" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="R14" s="72"/>
+      <c r="S14" s="71" t="s">
+        <v>57</v>
+      </c>
+      <c r="T14" s="78"/>
+      <c r="U14" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="V14" s="88"/>
+      <c r="X14" s="73"/>
+    </row>
+    <row r="15" spans="1:24" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="64"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="66" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="67" t="s">
         <v>66</v>
       </c>
-      <c r="J17" s="34"/>
-    </row>
-    <row r="18" spans="1:24" s="33" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="76"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="76"/>
-      <c r="L18" s="76"/>
-      <c r="M18" s="76"/>
-      <c r="N18" s="76"/>
-      <c r="O18" s="76"/>
-      <c r="P18" s="82"/>
-      <c r="Q18" s="82"/>
-      <c r="R18" s="82"/>
-      <c r="S18" s="76"/>
-      <c r="T18" s="76"/>
-      <c r="U18" s="82"/>
-      <c r="V18" s="82"/>
-    </row>
-    <row r="19" spans="1:24" s="94" customFormat="1" ht="12" x14ac:dyDescent="0.15">
-      <c r="A19" s="85" t="s">
-        <v>73</v>
-      </c>
-      <c r="B19" s="86"/>
-      <c r="C19" s="87"/>
-      <c r="D19" s="88" t="s">
-        <v>69</v>
-      </c>
-      <c r="E19" s="89" t="s">
-        <v>72</v>
-      </c>
-      <c r="F19" s="88" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" s="90" t="s">
-        <v>74</v>
-      </c>
-      <c r="H19" s="91"/>
-      <c r="I19" s="88" t="s">
-        <v>70</v>
-      </c>
-      <c r="J19" s="85" t="s">
+      <c r="F15" s="82" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="K19" s="92"/>
-      <c r="L19" s="86"/>
-      <c r="M19" s="87"/>
-      <c r="N19" s="85" t="s">
-        <v>38</v>
-      </c>
-      <c r="O19" s="86"/>
-      <c r="P19" s="93"/>
-      <c r="Q19" s="85" t="s">
-        <v>39</v>
-      </c>
-      <c r="R19" s="86"/>
-      <c r="S19" s="85" t="s">
+      <c r="H15" s="65"/>
+      <c r="I15" s="81" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="T19" s="92"/>
-      <c r="U19" s="85" t="s">
-        <v>71</v>
-      </c>
-      <c r="V19" s="93"/>
-      <c r="X19" s="87"/>
-    </row>
-    <row r="20" spans="1:24" s="71" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="68"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="68"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="68"/>
-      <c r="K20" s="70"/>
-      <c r="M20" s="70"/>
-    </row>
-    <row r="21" spans="1:24" s="72" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="77" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="78"/>
-      <c r="C21" s="79"/>
-      <c r="D21" s="80" t="s">
-        <v>58</v>
-      </c>
-      <c r="E21" s="81" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" s="96" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="81" t="s">
-        <v>78</v>
-      </c>
-      <c r="H21" s="79"/>
-      <c r="I21" s="95" t="s">
-        <v>59</v>
-      </c>
-      <c r="J21" s="81" t="s">
-        <v>77</v>
-      </c>
-      <c r="K21" s="78"/>
-      <c r="L21" s="78"/>
-      <c r="M21" s="79"/>
-      <c r="N21" s="81" t="s">
-        <v>60</v>
-      </c>
-      <c r="O21" s="78"/>
-      <c r="P21" s="79"/>
-      <c r="Q21" s="77" t="s">
-        <v>65</v>
-      </c>
-      <c r="R21" s="78"/>
-      <c r="S21" s="84" t="s">
-        <v>62</v>
-      </c>
-      <c r="T21" s="78"/>
-      <c r="U21" s="83" t="s">
-        <v>61</v>
-      </c>
-      <c r="V21" s="79"/>
-      <c r="X21" s="79"/>
-    </row>
-    <row r="22" spans="1:24" s="72" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="72" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="68"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="73"/>
-      <c r="J22" s="75"/>
-      <c r="K22" s="73"/>
-      <c r="L22" s="74"/>
-      <c r="M22" s="73"/>
-      <c r="N22" s="74"/>
-      <c r="O22" s="68"/>
-      <c r="W22"/>
-    </row>
-    <row r="23" spans="1:24" s="72" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="72" t="s">
-        <v>63</v>
-      </c>
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="73"/>
-      <c r="J23" s="75"/>
-      <c r="K23" s="73"/>
-      <c r="L23" s="74"/>
-      <c r="M23" s="73"/>
-      <c r="N23" s="74"/>
-      <c r="O23" s="68"/>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="E24" s="1"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="65"/>
+      <c r="N15" s="67" t="s">
+        <v>52</v>
+      </c>
+      <c r="O15" s="64"/>
+      <c r="P15" s="65"/>
+      <c r="Q15" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="R15" s="64"/>
+      <c r="S15" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="T15" s="64"/>
+      <c r="U15" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="V15" s="89"/>
+      <c r="X15" s="65"/>
+    </row>
+    <row r="16" spans="1:24" s="14" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="B16" s="15"/>
+      <c r="D16" s="27"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="V16" s="90"/>
+    </row>
+    <row r="17" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="1"/>
+      <c r="M17"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="1"/>
+      <c r="R17"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="12"/>
+    </row>
+    <row r="18" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="F18" s="1"/>
+      <c r="U18" s="12"/>
+    </row>
+    <row r="19" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="F19" s="1"/>
+      <c r="U19" s="12"/>
+    </row>
+    <row r="20" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="F20" s="1"/>
+      <c r="U20" s="12"/>
+    </row>
+    <row r="21" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="F21" s="1"/>
+      <c r="U21" s="12"/>
+    </row>
+    <row r="22" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="F22" s="1"/>
+      <c r="U22" s="12"/>
+    </row>
+    <row r="23" spans="4:21" x14ac:dyDescent="0.2">
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="1"/>
+      <c r="U23" s="12"/>
+    </row>
+    <row r="24" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F24" s="1"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="1"/>
-      <c r="M24"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="1"/>
-      <c r="R24"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="13"/>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="U24" s="12"/>
+    </row>
+    <row r="25" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F25" s="1"/>
-      <c r="U25" s="13"/>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="U25" s="12"/>
+    </row>
+    <row r="26" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F26" s="1"/>
-      <c r="U26" s="13"/>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.15">
+    </row>
+    <row r="27" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F27" s="1"/>
-      <c r="U27" s="13"/>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.15">
+    </row>
+    <row r="28" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F28" s="1"/>
-      <c r="U28" s="13"/>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.15">
+    </row>
+    <row r="29" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F29" s="1"/>
-      <c r="U29" s="13"/>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
+    </row>
+    <row r="30" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F30" s="1"/>
-      <c r="U30" s="13"/>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.15">
+    </row>
+    <row r="31" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F31" s="1"/>
-      <c r="U31" s="13"/>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.15">
+    </row>
+    <row r="32" spans="4:21" x14ac:dyDescent="0.2">
       <c r="F32" s="1"/>
-      <c r="U32" s="13"/>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.15">
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="40" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="41" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F42" s="1"/>
     </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="43" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F43" s="1"/>
     </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="44" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="45" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="46" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F46" s="1"/>
     </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="47" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="48" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F48" s="1"/>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F49" s="1"/>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F50" s="1"/>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="59" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="60" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="61" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F61" s="1"/>
     </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="62" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="63" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="64" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F64" s="1"/>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F65" s="1"/>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F66" s="1"/>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F67" s="1"/>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F68" s="1"/>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="69" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F69" s="1"/>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F70" s="1"/>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F71" s="1"/>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F72" s="1"/>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="73" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F73" s="1"/>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="74" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F74" s="1"/>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="75" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="76" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F76" s="1"/>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="77" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F77" s="1"/>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="78" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F78" s="1"/>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="79" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F79" s="1"/>
     </row>
-    <row r="80" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="80" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F80" s="1"/>
     </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="81" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F81" s="1"/>
     </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F82" s="1"/>
     </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="83" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F83" s="1"/>
     </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="84" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F84" s="1"/>
     </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="85" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F85" s="1"/>
     </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="86" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F86" s="1"/>
     </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="87" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F87" s="1"/>
     </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="88" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F88" s="1"/>
     </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="89" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F89" s="1"/>
     </row>
-    <row r="90" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="90" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F90" s="1"/>
     </row>
-    <row r="91" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="91" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F91" s="1"/>
     </row>
-    <row r="92" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="92" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F92" s="1"/>
     </row>
-    <row r="93" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="93" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F93" s="1"/>
     </row>
-    <row r="94" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="94" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F94" s="1"/>
     </row>
-    <row r="95" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="95" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F95" s="1"/>
     </row>
-    <row r="96" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="96" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="97" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F97" s="1"/>
     </row>
-    <row r="98" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="98" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F98" s="1"/>
     </row>
-    <row r="99" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="99" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F99" s="1"/>
     </row>
-    <row r="100" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="100" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F100" s="1"/>
     </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="101" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F101" s="1"/>
     </row>
-    <row r="102" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="102" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F102" s="1"/>
     </row>
-    <row r="103" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="103" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F103" s="1"/>
     </row>
-    <row r="104" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="104" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="105" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="106" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="107" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="108" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="109" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F109" s="1"/>
     </row>
-    <row r="110" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="110" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="111" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="112" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="113" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F113" s="1"/>
     </row>
-    <row r="114" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="114" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F114" s="1"/>
     </row>
-    <row r="115" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="115" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="116" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F116" s="1"/>
     </row>
-    <row r="117" spans="6:6" x14ac:dyDescent="0.15">
+    <row r="117" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F117" s="1"/>
-    </row>
-    <row r="118" spans="6:6" x14ac:dyDescent="0.15">
-      <c r="F118" s="1"/>
-    </row>
-    <row r="119" spans="6:6" x14ac:dyDescent="0.15">
-      <c r="F119" s="1"/>
-    </row>
-    <row r="120" spans="6:6" x14ac:dyDescent="0.15">
-      <c r="F120" s="1"/>
-    </row>
-    <row r="121" spans="6:6" x14ac:dyDescent="0.15">
-      <c r="F121" s="1"/>
-    </row>
-    <row r="122" spans="6:6" x14ac:dyDescent="0.15">
-      <c r="F122" s="1"/>
-    </row>
-    <row r="123" spans="6:6" x14ac:dyDescent="0.15">
-      <c r="F123" s="1"/>
-    </row>
-    <row r="124" spans="6:6" x14ac:dyDescent="0.15">
-      <c r="F124" s="1"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E10:F10"/>
     <mergeCell ref="K3:O3"/>
+    <mergeCell ref="K1:V1"/>
     <mergeCell ref="U6:U7"/>
     <mergeCell ref="V6:V7"/>
     <mergeCell ref="T6:T7"/>
@@ -2657,44 +2542,28 @@
     <mergeCell ref="O6:Q6"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:D8">
-    <cfRule type="expression" dxfId="6" priority="3" stopIfTrue="1">
-      <formula>AND((#REF!),#REF!,#REF!)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="7" stopIfTrue="1">
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9:D9">
-    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
-      <formula>AND((#REF!),#REF!,#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C20:D20">
-    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
-      <formula>AND((#REF!),#REF!,#REF!)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
-      <formula>AND((#REF!),#REF!,#REF!)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12:E12 D13:F13">
+  <conditionalFormatting sqref="D10:E10">
     <cfRule type="expression" dxfId="1" priority="11" stopIfTrue="1">
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:F18">
+  <conditionalFormatting sqref="D11:F13">
     <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
       <formula>AND((#REF!),#REF!,#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation showErrorMessage="1" sqref="K4" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="H12" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" sqref="H13:H18" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation allowBlank="1" showErrorMessage="1" sqref="H10" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" sqref="H11:H13" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8:I9 H20" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I8" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>0</formula1>
       <formula2>200</formula2>
     </dataValidation>
@@ -2703,8 +2572,9 @@
     <hyperlink ref="A3" r:id="rId1" display="www.federation.org" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="A4" r:id="rId2" display="records@federation.org" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
-  <pageMargins left="0.31496062992125984" right="0.35433070866141736" top="0.39370078740157483" bottom="0.47244094488188981" header="0.51181102362204722" footer="0.23622047244094491"/>
+  <pageMargins left="0.31496062992125984" right="0.35433070866141736" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="70" firstPageNumber="0" fitToHeight="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
   <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>